<commit_message>
Added some edb data
</commit_message>
<xml_diff>
--- a/analysis_2022/data_raw/ToxinResults_Barriersampling_EH.xlsx
+++ b/analysis_2022/data_raw/ToxinResults_Barriersampling_EH.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater.sharepoint.com/teams/DWR-EXT-PROJ-2021-Emer-Drought-Barrier-Report/Shared Documents/General/Biological/DWR HAB sampling/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/cpien_usbr_gov/Documents/Work/HAB/EDB-HABs-Weeds/analysis_2022/data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="8_{9207360D-BDED-4C1C-9147-8C09EF08306F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B5B6859-F982-4B28-8507-0BEFE5F805A8}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="8_{9207360D-BDED-4C1C-9147-8C09EF08306F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1AA01C18-EDA5-4978-8C84-F26A74F3FFFF}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{C4D24093-7595-43F7-AA3C-36DDE7CF8AED}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{C4D24093-7595-43F7-AA3C-36DDE7CF8AED}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="103">
   <si>
     <t>Station</t>
   </si>
@@ -719,27 +719,27 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7265625" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -747,7 +747,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -755,7 +755,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -763,7 +763,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -771,7 +771,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -779,7 +779,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -787,7 +787,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -795,7 +795,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -803,12 +803,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -816,7 +816,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -824,7 +824,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -832,7 +832,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -840,7 +840,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -848,7 +848,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>60</v>
       </c>
@@ -856,7 +856,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>65</v>
       </c>
@@ -874,13 +874,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A758DC6-C613-47B0-AEE2-275944784EC9}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>94</v>
       </c>
@@ -894,7 +897,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -908,7 +911,7 @@
         <v>-121.667123</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -922,7 +925,7 @@
         <v>-121.5981</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -936,7 +939,7 @@
         <v>-121.51093299999999</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -950,7 +953,7 @@
         <v>-121.58212399999999</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -977,16 +980,16 @@
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.26953125" customWidth="1"/>
-    <col min="3" max="3" width="17.1796875" customWidth="1"/>
-    <col min="4" max="5" width="13.81640625" customWidth="1"/>
-    <col min="6" max="6" width="22.54296875" customWidth="1"/>
-    <col min="7" max="7" width="18.453125" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1012,7 +1015,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1035,7 +1038,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1058,7 +1061,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1081,7 +1084,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1104,7 +1107,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1127,7 +1130,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1150,7 +1153,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1176,7 +1179,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1199,7 +1202,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1225,7 +1228,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1251,7 +1254,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1274,7 +1277,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1297,7 +1300,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1323,7 +1326,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1349,7 +1352,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1375,7 +1378,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1401,7 +1404,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1427,7 +1430,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -1453,7 +1456,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -1479,7 +1482,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -1505,7 +1508,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -1531,7 +1534,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -1557,7 +1560,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -1583,7 +1586,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -1609,7 +1612,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>51</v>
       </c>
@@ -1635,7 +1638,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -1661,7 +1664,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>51</v>
       </c>
@@ -1687,7 +1690,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -1713,7 +1716,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -1739,7 +1742,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -1765,7 +1768,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -1791,7 +1794,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -1817,7 +1820,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -1843,7 +1846,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -1869,7 +1872,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>15</v>
       </c>
@@ -1895,7 +1898,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>15</v>
       </c>
@@ -1921,7 +1924,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -1947,7 +1950,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -1973,7 +1976,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -1999,7 +2002,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
     </row>
   </sheetData>
@@ -2009,21 +2012,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC6F3B63-CA45-43DA-A3B5-737AF56B3AA6}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.7265625" customWidth="1"/>
-    <col min="3" max="3" width="16.453125" customWidth="1"/>
-    <col min="4" max="5" width="12.54296875" customWidth="1"/>
-    <col min="6" max="6" width="15.81640625" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2046,7 +2049,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2069,7 +2072,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2092,7 +2095,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2115,7 +2118,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -2138,7 +2141,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -2161,7 +2164,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -2184,7 +2187,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -2207,7 +2210,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -2230,7 +2233,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -2253,7 +2256,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -2276,7 +2279,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -2299,7 +2302,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -2322,7 +2325,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -2345,7 +2348,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -2368,7 +2371,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -2391,7 +2394,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -2414,7 +2417,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -2437,7 +2440,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -2460,7 +2463,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -2483,7 +2486,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -2506,7 +2509,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -2529,7 +2532,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -2552,7 +2555,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -2575,7 +2578,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -2598,7 +2601,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -2621,7 +2624,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -2642,6 +2645,22 @@
       </c>
       <c r="G27">
         <v>0.05</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="1">
+        <v>44812</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="1">
+        <v>44824</v>
       </c>
     </row>
   </sheetData>
@@ -2651,6 +2670,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="ce32806a-8640-4bdf-8dde-24791ef51772">
@@ -2659,15 +2687,6 @@
     <TaxCatchAll xmlns="7d8e2b3b-bd99-497c-a4aa-8b1943090515" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2900,20 +2919,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F6E5BC-80D0-4A43-9AA1-C41459911231}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23E0C704-4ADD-4CA7-96EC-18677C653A66}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="ce32806a-8640-4bdf-8dde-24791ef51772"/>
     <ds:schemaRef ds:uri="7d8e2b3b-bd99-497c-a4aa-8b1943090515"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F6E5BC-80D0-4A43-9AA1-C41459911231}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updated ptox data and plots
</commit_message>
<xml_diff>
--- a/analysis_2022/data_raw/ToxinResults_Barriersampling_EH.xlsx
+++ b/analysis_2022/data_raw/ToxinResults_Barriersampling_EH.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/cpien_usbr_gov/Documents/Work/HAB/EDB-HABs-Weeds/analysis_2022/data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="8_{9207360D-BDED-4C1C-9147-8C09EF08306F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1AA01C18-EDA5-4978-8C84-F26A74F3FFFF}"/>
+  <xr:revisionPtr revIDLastSave="187" documentId="8_{9207360D-BDED-4C1C-9147-8C09EF08306F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1360745B-5E78-43CA-AD00-F86DCA5FACCB}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{C4D24093-7595-43F7-AA3C-36DDE7CF8AED}"/>
+    <workbookView xWindow="6390" yWindow="2475" windowWidth="21600" windowHeight="11265" activeTab="2" xr2:uid="{C4D24093-7595-43F7-AA3C-36DDE7CF8AED}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="118">
   <si>
     <t>Station</t>
   </si>
@@ -346,13 +346,102 @@
   </si>
   <si>
     <t>Old River at Holt</t>
+  </si>
+  <si>
+    <t>FAL_SG_221025</t>
+  </si>
+  <si>
+    <t>DUP_SG_221025</t>
+  </si>
+  <si>
+    <t>HOL_SG_221013</t>
+  </si>
+  <si>
+    <t>The PTOX cyanobacterium cf. Phormidium sp. (~1 filament per mL) was observed.</t>
+  </si>
+  <si>
+    <t>HLT_SG_221013</t>
+  </si>
+  <si>
+    <t>DUP_SG_221013</t>
+  </si>
+  <si>
+    <t>FAL_SG_220926</t>
+  </si>
+  <si>
+    <t>DUP_SG_220926</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The PTOX cyanobacteria </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Microcystis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sp. (1 colonly per mL) and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Aphanizomenon </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sp. (2 filaments per mL) were observed.</t>
+    </r>
+  </si>
+  <si>
+    <t>HOL_SG_220908</t>
+  </si>
+  <si>
+    <t>HLT_SG_220908</t>
+  </si>
+  <si>
+    <t>DUP_SG_220908</t>
+  </si>
+  <si>
+    <t>The PTOX cyanobacteria Planktothrix sp. (3 filaments per mL) and 1 nostocalean filament per mL were observed. Specialized cells (i.e. akinetes, heterocytes) were not present on the nostocalean filament, preventing genus level identification.</t>
+  </si>
+  <si>
+    <t>FAL_SG_2020831</t>
+  </si>
+  <si>
+    <t>DUP_SG_2020831</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -368,6 +457,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -974,10 +1071,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33168318-33C0-4102-8E85-BB0086D8E249}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2003,19 +2100,334 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="1"/>
+      <c r="A41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="1">
+        <v>44859</v>
+      </c>
+      <c r="C41" t="s">
+        <v>103</v>
+      </c>
+      <c r="D41" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" t="s">
+        <v>11</v>
+      </c>
+      <c r="G41" t="s">
+        <v>8</v>
+      </c>
+      <c r="H41" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42" s="1">
+        <v>44859</v>
+      </c>
+      <c r="C42" t="s">
+        <v>104</v>
+      </c>
+      <c r="D42" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" t="s">
+        <v>8</v>
+      </c>
+      <c r="H42" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" s="1">
+        <v>44847</v>
+      </c>
+      <c r="C43" t="s">
+        <v>105</v>
+      </c>
+      <c r="D43" t="s">
+        <v>72</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43" t="s">
+        <v>11</v>
+      </c>
+      <c r="G43" t="s">
+        <v>8</v>
+      </c>
+      <c r="H43" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>15</v>
+      </c>
+      <c r="B44" s="1">
+        <v>44847</v>
+      </c>
+      <c r="C44" t="s">
+        <v>107</v>
+      </c>
+      <c r="D44" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" t="s">
+        <v>11</v>
+      </c>
+      <c r="G44" t="s">
+        <v>8</v>
+      </c>
+      <c r="H44" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>15</v>
+      </c>
+      <c r="B45" s="1">
+        <v>44847</v>
+      </c>
+      <c r="C45" t="s">
+        <v>108</v>
+      </c>
+      <c r="D45" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" t="s">
+        <v>8</v>
+      </c>
+      <c r="H45" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" s="1">
+        <v>44830</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D46" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46" t="s">
+        <v>11</v>
+      </c>
+      <c r="G46" t="s">
+        <v>8</v>
+      </c>
+      <c r="H46" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="1">
+        <v>44830</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D47" t="s">
+        <v>41</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47" t="s">
+        <v>11</v>
+      </c>
+      <c r="G47" t="s">
+        <v>8</v>
+      </c>
+      <c r="H47" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>19</v>
+      </c>
+      <c r="B48" s="1">
+        <v>44830</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D48" t="s">
+        <v>33</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+      <c r="F48" t="s">
+        <v>11</v>
+      </c>
+      <c r="G48" t="s">
+        <v>8</v>
+      </c>
+      <c r="H48" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" s="1">
+        <v>44812</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D49" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49" t="s">
+        <v>11</v>
+      </c>
+      <c r="G49" t="s">
+        <v>8</v>
+      </c>
+      <c r="H49" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>15</v>
+      </c>
+      <c r="B50" s="1">
+        <v>44812</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D50" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" t="s">
+        <v>11</v>
+      </c>
+      <c r="G50" t="s">
+        <v>8</v>
+      </c>
+      <c r="H50" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51" s="1">
+        <v>44812</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D51" t="s">
+        <v>49</v>
+      </c>
+      <c r="E51">
+        <v>3</v>
+      </c>
+      <c r="F51" t="s">
+        <v>11</v>
+      </c>
+      <c r="G51" t="s">
+        <v>8</v>
+      </c>
+      <c r="H51" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>19</v>
+      </c>
+      <c r="B52" s="1">
+        <v>44804</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D52" t="s">
+        <v>49</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52" t="s">
+        <v>11</v>
+      </c>
+      <c r="G52" t="s">
+        <v>8</v>
+      </c>
+      <c r="H52" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>19</v>
+      </c>
+      <c r="B53" s="1">
+        <v>44804</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D53" t="s">
+        <v>49</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53" t="s">
+        <v>11</v>
+      </c>
+      <c r="G53" t="s">
+        <v>8</v>
+      </c>
+      <c r="H53" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC6F3B63-CA45-43DA-A3B5-737AF56B3AA6}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:G17"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2647,22 +3059,6 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="1">
-        <v>44812</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>51</v>
-      </c>
-      <c r="B29" s="1">
-        <v>44824</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2670,26 +3066,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ce32806a-8640-4bdf-8dde-24791ef51772">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7d8e2b3b-bd99-497c-a4aa-8b1943090515" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010047BDD1B75669E94AB690344454A2FDA0" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fc0869692887afc2ca9e8ccef3644641">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ce32806a-8640-4bdf-8dde-24791ef51772" xmlns:ns3="7d8e2b3b-bd99-497c-a4aa-8b1943090515" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="014a6ad56f10121cfc7dede17ba95b52" ns2:_="" ns3:_="">
     <xsd:import namespace="ce32806a-8640-4bdf-8dde-24791ef51772"/>
@@ -2918,10 +3294,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ce32806a-8640-4bdf-8dde-24791ef51772">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7d8e2b3b-bd99-497c-a4aa-8b1943090515" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F6E5BC-80D0-4A43-9AA1-C41459911231}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F24CAD53-EDE9-4F5E-8887-919B43745176}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ce32806a-8640-4bdf-8dde-24791ef51772"/>
+    <ds:schemaRef ds:uri="7d8e2b3b-bd99-497c-a4aa-8b1943090515"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2938,20 +3345,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F24CAD53-EDE9-4F5E-8887-919B43745176}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F6E5BC-80D0-4A43-9AA1-C41459911231}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ce32806a-8640-4bdf-8dde-24791ef51772"/>
-    <ds:schemaRef ds:uri="7d8e2b3b-bd99-497c-a4aa-8b1943090515"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>